<commit_message>
[Documentation] Weekly Report - 2
</commit_message>
<xml_diff>
--- a/Documentation/Project Weekly Report - FHF - 1.xlsx
+++ b/Documentation/Project Weekly Report - FHF - 1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85301ABB-7E43-4009-A40B-15DE006F36BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F06A11A-A802-4063-951A-0A0FD8F107FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>chốt đề tài</t>
   </si>
   <si>
     <t>SEP490_G1</t>
@@ -708,11 +705,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +732,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -743,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -773,10 +770,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -788,16 +785,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -805,16 +802,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -822,10 +819,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -855,30 +852,30 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -889,147 +886,145 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>5</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="9">
+        <v>44874</v>
+      </c>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>1</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="9">
-        <v>44874</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1053,16 +1048,9 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D16 D6:D9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D15 D6:D9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pending, In Progress, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>